<commit_message>
lots of new gonad plots, new scripts
</commit_message>
<xml_diff>
--- a/Data/RNA-DNA-Isolation/DNA-extraction-data.xlsx
+++ b/Data/RNA-DNA-Isolation/DNA-extraction-data.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28331"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11109"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laura/Documents/roberts-lab/O.lurida_Stress/Data/RNA-DNA-Isolation/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7177B820-9CB2-F041-93F1-D4B2302371B1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="0" windowWidth="25520" windowHeight="15280" tabRatio="1000" activeTab="1"/>
+    <workbookView xWindow="14500" yWindow="460" windowWidth="13640" windowHeight="17100" tabRatio="1000" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DNA Samples" sheetId="1" r:id="rId1"/>
@@ -14,10 +20,10 @@
     <sheet name="QubitData_2018-03-10_01-06-26.c" sheetId="3" r:id="rId5"/>
     <sheet name="QubitData_2018-03-13_Larvae-DNA" sheetId="5" r:id="rId6"/>
     <sheet name="QubitData_2018-03-27_Gonad-RNA" sheetId="7" r:id="rId7"/>
-    <sheet name="QubitData_2018-04-02_11-21-01.c" sheetId="8" r:id="rId8"/>
+    <sheet name="QubitData_2018-04-02_Larval-RNA" sheetId="8" r:id="rId8"/>
     <sheet name="Samples sent for QuantSeq" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,12 +33,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Laura Spencer</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000001000000}">
       <text>
         <r>
           <rPr>
@@ -48,7 +54,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000002000000}">
       <text>
         <r>
           <rPr>
@@ -73,7 +79,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A14" authorId="0">
+    <comment ref="A14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0800-000003000000}">
       <text>
         <r>
           <rPr>
@@ -103,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1500" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1533" uniqueCount="364">
   <si>
     <t>SAMPLE #</t>
   </si>
@@ -1174,6 +1180,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> or 67-A</t>
@@ -1210,16 +1217,23 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> or 67-A</t>
     </r>
   </si>
+  <si>
+    <t>Spawning-Group</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -1282,6 +1296,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1302,6 +1317,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1317,6 +1333,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1324,12 +1341,14 @@
       <sz val="12"/>
       <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1338,6 +1357,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1346,6 +1366,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1364,6 +1385,7 @@
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1371,6 +1393,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -2307,8 +2330,8 @@
   </cellXfs>
   <cellStyles count="505">
     <cellStyle name="Comma" xfId="81" builtinId="3"/>
-    <cellStyle name="Comma 2" xfId="175"/>
-    <cellStyle name="Comma 3" xfId="414"/>
+    <cellStyle name="Comma 2" xfId="175" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Comma 3" xfId="414" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2814,6 +2837,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -3138,14 +3169,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q58"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView showRuler="0" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="L58" sqref="L58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.33203125" style="11" customWidth="1"/>
     <col min="2" max="3" width="10.83203125" style="11" customWidth="1"/>
@@ -3164,7 +3195,7 @@
     <col min="18" max="16384" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="8" customFormat="1" ht="45">
+    <row r="1" spans="1:17" s="8" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>69</v>
       </c>
@@ -3217,7 +3248,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>20</v>
       </c>
@@ -3258,7 +3289,7 @@
         <v>4.7119999999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>21</v>
       </c>
@@ -3299,7 +3330,7 @@
         <v>7.258</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>22</v>
       </c>
@@ -3340,7 +3371,7 @@
         <v>1.5352000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>23</v>
       </c>
@@ -3381,7 +3412,7 @@
         <v>17.081000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>31</v>
       </c>
@@ -3425,7 +3456,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>32</v>
       </c>
@@ -3466,7 +3497,7 @@
         <v>6.5940000000000012</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>33</v>
       </c>
@@ -3507,7 +3538,7 @@
         <v>2.4360000000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>34</v>
       </c>
@@ -3548,7 +3579,7 @@
         <v>1.5864000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>30</v>
       </c>
@@ -3581,7 +3612,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>35</v>
       </c>
@@ -3614,7 +3645,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>36</v>
       </c>
@@ -3647,7 +3678,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>37</v>
       </c>
@@ -3680,7 +3711,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>47</v>
       </c>
@@ -3719,7 +3750,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
         <v>70</v>
       </c>
@@ -3754,7 +3785,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>71</v>
       </c>
@@ -3789,7 +3820,7 @@
         <v>22.990000000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
         <v>50</v>
       </c>
@@ -3824,7 +3855,7 @@
         <v>10.450000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
         <v>51</v>
       </c>
@@ -3859,7 +3890,7 @@
         <v>24.225000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
         <v>52</v>
       </c>
@@ -3894,7 +3925,7 @@
         <v>21.66</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>53</v>
       </c>
@@ -3929,7 +3960,7 @@
         <v>11.742000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>63</v>
       </c>
@@ -3964,7 +3995,7 @@
         <v>19.9025</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>64</v>
       </c>
@@ -3999,7 +4030,7 @@
         <v>8.8919999999999995</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
         <v>48</v>
       </c>
@@ -4026,7 +4057,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>49</v>
       </c>
@@ -4053,7 +4084,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
         <v>73</v>
       </c>
@@ -4080,7 +4111,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="28" customHeight="1">
+    <row r="27" spans="1:16" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
         <v>153</v>
       </c>
@@ -4128,7 +4159,7 @@
         <v>70.5</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="28" customHeight="1">
+    <row r="28" spans="1:16" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
         <v>154</v>
       </c>
@@ -4170,7 +4201,7 @@
         <v>23.5</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="28" customHeight="1">
+    <row r="29" spans="1:16" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
         <v>154</v>
       </c>
@@ -4212,7 +4243,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="28" customHeight="1">
+    <row r="30" spans="1:16" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
         <v>155</v>
       </c>
@@ -4260,7 +4291,7 @@
         <v>79.125</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="28" customHeight="1">
+    <row r="31" spans="1:16" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
         <v>156</v>
       </c>
@@ -4302,7 +4333,7 @@
         <v>21.25</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="28" customHeight="1">
+    <row r="32" spans="1:16" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>157</v>
       </c>
@@ -4344,7 +4375,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="28" customHeight="1">
+    <row r="33" spans="1:16" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
         <v>158</v>
       </c>
@@ -4392,7 +4423,7 @@
         <v>103.125</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="28" customHeight="1">
+    <row r="34" spans="1:16" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
         <v>159</v>
       </c>
@@ -4434,7 +4465,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="28" customHeight="1">
+    <row r="35" spans="1:16" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
         <v>160</v>
       </c>
@@ -4476,7 +4507,7 @@
         <v>31.875</v>
       </c>
     </row>
-    <row r="36" spans="1:16" ht="28" customHeight="1">
+    <row r="36" spans="1:16" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
         <v>161</v>
       </c>
@@ -4524,7 +4555,7 @@
         <v>111.25</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="28" customHeight="1">
+    <row r="37" spans="1:16" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
         <v>162</v>
       </c>
@@ -4566,7 +4597,7 @@
         <v>36.875</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="28" customHeight="1">
+    <row r="38" spans="1:16" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
         <v>163</v>
       </c>
@@ -4608,7 +4639,7 @@
         <v>37.5</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="28" customHeight="1">
+    <row r="39" spans="1:16" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
         <v>164</v>
       </c>
@@ -4656,7 +4687,7 @@
         <v>92.5</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="28" customHeight="1">
+    <row r="40" spans="1:16" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
         <v>165</v>
       </c>
@@ -4698,7 +4729,7 @@
         <v>29.375</v>
       </c>
     </row>
-    <row r="41" spans="1:16" ht="28" customHeight="1">
+    <row r="41" spans="1:16" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
         <v>166</v>
       </c>
@@ -4740,7 +4771,7 @@
         <v>33.75</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="28" customHeight="1">
+    <row r="42" spans="1:16" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
         <v>167</v>
       </c>
@@ -4788,7 +4819,7 @@
         <v>99.3125</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="28" customHeight="1">
+    <row r="43" spans="1:16" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
         <v>168</v>
       </c>
@@ -4830,7 +4861,7 @@
         <v>35.250000000000007</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="28" customHeight="1">
+    <row r="44" spans="1:16" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="s">
         <v>169</v>
       </c>
@@ -4872,7 +4903,7 @@
         <v>30.9375</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="28" customHeight="1">
+    <row r="45" spans="1:16" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
         <v>170</v>
       </c>
@@ -4920,7 +4951,7 @@
         <v>89.0625</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="28" customHeight="1">
+    <row r="46" spans="1:16" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
         <v>171</v>
       </c>
@@ -4962,7 +4993,7 @@
         <v>27.5</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="28" customHeight="1">
+    <row r="47" spans="1:16" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
         <v>172</v>
       </c>
@@ -5004,7 +5035,7 @@
         <v>29.6875</v>
       </c>
     </row>
-    <row r="48" spans="1:16" ht="28" customHeight="1">
+    <row r="48" spans="1:16" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
         <v>173</v>
       </c>
@@ -5052,7 +5083,7 @@
         <v>104.9375</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="28" customHeight="1">
+    <row r="49" spans="1:15" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="11" t="s">
         <v>174</v>
       </c>
@@ -5094,7 +5125,7 @@
         <v>35.062499999999993</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="28" customHeight="1">
+    <row r="50" spans="1:15" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
         <v>175</v>
       </c>
@@ -5136,7 +5167,7 @@
         <v>33.000000000000007</v>
       </c>
     </row>
-    <row r="51" spans="1:15">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B51" s="11" t="s">
         <v>146</v>
       </c>
@@ -5153,7 +5184,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="52" spans="1:15">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B52" s="11" t="s">
         <v>148</v>
       </c>
@@ -5170,7 +5201,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="53" spans="1:15">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B53" s="11" t="s">
         <v>138</v>
       </c>
@@ -5187,7 +5218,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="54" spans="1:15">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B54" s="11" t="s">
         <v>150</v>
       </c>
@@ -5204,7 +5235,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="1:15">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B55" s="11" t="s">
         <v>152</v>
       </c>
@@ -5221,7 +5252,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:15">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B56" s="11" t="s">
         <v>145</v>
       </c>
@@ -5238,7 +5269,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:15">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B57" s="11" t="s">
         <v>147</v>
       </c>
@@ -5255,7 +5286,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="1:15">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E58" s="16"/>
     </row>
   </sheetData>
@@ -5275,17 +5306,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="M63" sqref="M63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.33203125" style="64" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
@@ -5303,7 +5334,7 @@
     <col min="14" max="14" width="31.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="66" customFormat="1" ht="42" customHeight="1">
+    <row r="1" spans="1:20" s="66" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>342</v>
       </c>
@@ -5345,7 +5376,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="2" spans="1:20" hidden="1">
+    <row r="2" spans="1:20" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="33"/>
       <c r="B2" s="11">
         <v>1</v>
@@ -5379,7 +5410,7 @@
       </c>
       <c r="M2" s="11"/>
     </row>
-    <row r="3" spans="1:20" s="46" customFormat="1">
+    <row r="3" spans="1:20" s="46" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="59" t="s">
         <v>341</v>
       </c>
@@ -5419,7 +5450,7 @@
       <c r="N3" s="79"/>
       <c r="P3" s="79"/>
     </row>
-    <row r="4" spans="1:20" s="30" customFormat="1">
+    <row r="4" spans="1:20" s="30" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="58" t="s">
         <v>341</v>
       </c>
@@ -5459,7 +5490,7 @@
       <c r="N4" s="34"/>
       <c r="P4" s="34"/>
     </row>
-    <row r="5" spans="1:20" s="23" customFormat="1" hidden="1">
+    <row r="5" spans="1:20" s="23" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="24"/>
       <c r="B5" s="24" t="s">
         <v>277</v>
@@ -5495,7 +5526,7 @@
       <c r="S5"/>
       <c r="T5"/>
     </row>
-    <row r="6" spans="1:20" s="30" customFormat="1" hidden="1">
+    <row r="6" spans="1:20" s="30" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="58"/>
       <c r="B6" s="27">
         <v>5</v>
@@ -5533,7 +5564,7 @@
       <c r="N6" s="34"/>
       <c r="P6" s="34"/>
     </row>
-    <row r="7" spans="1:20" s="50" customFormat="1" hidden="1">
+    <row r="7" spans="1:20" s="50" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="63"/>
       <c r="B7" s="47">
         <v>6</v>
@@ -5569,7 +5600,7 @@
       <c r="N7" s="77"/>
       <c r="P7" s="77"/>
     </row>
-    <row r="8" spans="1:20" s="30" customFormat="1">
+    <row r="8" spans="1:20" s="30" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="58" t="s">
         <v>341</v>
       </c>
@@ -5609,7 +5640,7 @@
       <c r="N8" s="34"/>
       <c r="P8" s="34"/>
     </row>
-    <row r="9" spans="1:20" ht="15" hidden="1" customHeight="1">
+    <row r="9" spans="1:20" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="33"/>
       <c r="B9" s="11">
         <v>8</v>
@@ -5645,7 +5676,7 @@
       <c r="N9" s="25"/>
       <c r="P9" s="25"/>
     </row>
-    <row r="10" spans="1:20" s="30" customFormat="1">
+    <row r="10" spans="1:20" s="30" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="58"/>
       <c r="B10" s="27">
         <v>9</v>
@@ -5683,7 +5714,7 @@
       <c r="N10" s="34"/>
       <c r="P10" s="34"/>
     </row>
-    <row r="11" spans="1:20" s="55" customFormat="1">
+    <row r="11" spans="1:20" s="55" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="60" t="s">
         <v>341</v>
       </c>
@@ -5723,7 +5754,7 @@
       <c r="N11" s="80"/>
       <c r="P11" s="80"/>
     </row>
-    <row r="12" spans="1:20" s="55" customFormat="1">
+    <row r="12" spans="1:20" s="55" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="60" t="s">
         <v>341</v>
       </c>
@@ -5763,7 +5794,7 @@
       <c r="N12" s="80"/>
       <c r="P12" s="80"/>
     </row>
-    <row r="13" spans="1:20" s="76" customFormat="1" hidden="1">
+    <row r="13" spans="1:20" s="76" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="72"/>
       <c r="B13" s="73">
         <v>12</v>
@@ -5799,7 +5830,7 @@
       <c r="N13" s="82"/>
       <c r="P13" s="82"/>
     </row>
-    <row r="14" spans="1:20" s="55" customFormat="1">
+    <row r="14" spans="1:20" s="55" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="60" t="s">
         <v>341</v>
       </c>
@@ -5839,7 +5870,7 @@
       <c r="N14" s="80"/>
       <c r="P14" s="80"/>
     </row>
-    <row r="15" spans="1:20" s="55" customFormat="1">
+    <row r="15" spans="1:20" s="55" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="60" t="s">
         <v>341</v>
       </c>
@@ -5879,7 +5910,7 @@
       <c r="N15" s="80"/>
       <c r="P15" s="80"/>
     </row>
-    <row r="16" spans="1:20" s="55" customFormat="1">
+    <row r="16" spans="1:20" s="55" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="60" t="s">
         <v>341</v>
       </c>
@@ -5919,7 +5950,7 @@
       <c r="N16" s="80"/>
       <c r="P16" s="80"/>
     </row>
-    <row r="17" spans="1:20" s="88" customFormat="1" hidden="1">
+    <row r="17" spans="1:20" s="88" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="81"/>
       <c r="B17" s="81" t="s">
         <v>277</v>
@@ -5955,7 +5986,7 @@
       <c r="S17" s="76"/>
       <c r="T17" s="76"/>
     </row>
-    <row r="18" spans="1:20" s="76" customFormat="1" hidden="1">
+    <row r="18" spans="1:20" s="76" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="72"/>
       <c r="B18" s="73">
         <v>17</v>
@@ -5991,7 +6022,7 @@
       <c r="N18" s="82"/>
       <c r="P18" s="82"/>
     </row>
-    <row r="19" spans="1:20" s="76" customFormat="1" hidden="1">
+    <row r="19" spans="1:20" s="76" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="72"/>
       <c r="B19" s="73">
         <v>18</v>
@@ -6027,7 +6058,7 @@
       <c r="N19" s="82"/>
       <c r="P19" s="82"/>
     </row>
-    <row r="20" spans="1:20" s="76" customFormat="1">
+    <row r="20" spans="1:20" s="76" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="72" t="s">
         <v>341</v>
       </c>
@@ -6066,7 +6097,7 @@
       <c r="N20" s="82"/>
       <c r="P20" s="82"/>
     </row>
-    <row r="21" spans="1:20" s="76" customFormat="1">
+    <row r="21" spans="1:20" s="76" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="72"/>
       <c r="B21" s="81" t="s">
         <v>277</v>
@@ -6103,7 +6134,7 @@
       <c r="N21" s="82"/>
       <c r="P21" s="82"/>
     </row>
-    <row r="22" spans="1:20" s="55" customFormat="1">
+    <row r="22" spans="1:20" s="55" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="60" t="s">
         <v>341</v>
       </c>
@@ -6143,7 +6174,7 @@
       <c r="N22" s="80"/>
       <c r="P22" s="80"/>
     </row>
-    <row r="23" spans="1:20" s="76" customFormat="1" hidden="1">
+    <row r="23" spans="1:20" s="76" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="72"/>
       <c r="B23" s="73">
         <v>20</v>
@@ -6179,7 +6210,7 @@
       <c r="N23" s="82"/>
       <c r="P23" s="82"/>
     </row>
-    <row r="24" spans="1:20" s="76" customFormat="1" hidden="1">
+    <row r="24" spans="1:20" s="76" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="72"/>
       <c r="B24" s="72" t="s">
         <v>277</v>
@@ -6216,7 +6247,7 @@
       <c r="N24" s="82"/>
       <c r="P24" s="82"/>
     </row>
-    <row r="25" spans="1:20" s="55" customFormat="1">
+    <row r="25" spans="1:20" s="55" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="60" t="s">
         <v>341</v>
       </c>
@@ -6256,7 +6287,7 @@
       <c r="N25" s="80"/>
       <c r="P25" s="80"/>
     </row>
-    <row r="26" spans="1:20" s="76" customFormat="1" hidden="1">
+    <row r="26" spans="1:20" s="76" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="72"/>
       <c r="B26" s="73">
         <v>22</v>
@@ -6287,7 +6318,7 @@
       <c r="N26" s="82"/>
       <c r="P26" s="82"/>
     </row>
-    <row r="27" spans="1:20" s="55" customFormat="1">
+    <row r="27" spans="1:20" s="55" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="60" t="s">
         <v>341</v>
       </c>
@@ -6327,7 +6358,7 @@
       <c r="N27" s="80"/>
       <c r="P27" s="80"/>
     </row>
-    <row r="28" spans="1:20" s="55" customFormat="1">
+    <row r="28" spans="1:20" s="55" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="60" t="s">
         <v>341</v>
       </c>
@@ -6367,7 +6398,7 @@
       <c r="N28" s="80"/>
       <c r="P28" s="80"/>
     </row>
-    <row r="29" spans="1:20" s="105" customFormat="1" hidden="1">
+    <row r="29" spans="1:20" s="105" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="99"/>
       <c r="B29" s="100"/>
       <c r="C29" s="101" t="s">
@@ -6407,7 +6438,7 @@
       <c r="S29" s="50"/>
       <c r="T29" s="50"/>
     </row>
-    <row r="30" spans="1:20" s="105" customFormat="1">
+    <row r="30" spans="1:20" s="105" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="107" t="s">
         <v>341</v>
       </c>
@@ -6449,7 +6480,7 @@
       <c r="S30" s="50"/>
       <c r="T30" s="50"/>
     </row>
-    <row r="31" spans="1:20" s="30" customFormat="1" hidden="1">
+    <row r="31" spans="1:20" s="30" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="58"/>
       <c r="B31" s="27">
         <v>27</v>
@@ -6487,7 +6518,7 @@
       <c r="N31" s="34"/>
       <c r="P31" s="34"/>
     </row>
-    <row r="32" spans="1:20" s="46" customFormat="1">
+    <row r="32" spans="1:20" s="46" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="59"/>
       <c r="B32" s="43">
         <v>28</v>
@@ -6525,7 +6556,7 @@
       <c r="N32" s="79"/>
       <c r="P32" s="79"/>
     </row>
-    <row r="33" spans="1:13" s="46" customFormat="1">
+    <row r="33" spans="1:13" s="46" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="59" t="s">
         <v>341</v>
       </c>
@@ -6563,7 +6594,7 @@
       </c>
       <c r="M33" s="43"/>
     </row>
-    <row r="34" spans="1:13" s="88" customFormat="1" hidden="1">
+    <row r="34" spans="1:13" s="88" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="81"/>
       <c r="B34" s="85"/>
       <c r="C34" s="84" t="s">
@@ -6590,7 +6621,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="35" spans="1:13" s="105" customFormat="1">
+    <row r="35" spans="1:13" s="105" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="99"/>
       <c r="B35" s="100"/>
       <c r="C35" s="101" t="s">
@@ -6621,7 +6652,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="36" spans="1:13" s="76" customFormat="1" hidden="1">
+    <row r="36" spans="1:13" s="76" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="72"/>
       <c r="B36" s="73">
         <v>32</v>
@@ -6655,7 +6686,7 @@
       </c>
       <c r="M36" s="73"/>
     </row>
-    <row r="37" spans="1:13" s="46" customFormat="1">
+    <row r="37" spans="1:13" s="46" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="59" t="s">
         <v>341</v>
       </c>
@@ -6693,7 +6724,7 @@
       </c>
       <c r="M37" s="43"/>
     </row>
-    <row r="38" spans="1:13" s="55" customFormat="1">
+    <row r="38" spans="1:13" s="55" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="60" t="s">
         <v>341</v>
       </c>
@@ -6733,7 +6764,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="39" spans="1:13" s="55" customFormat="1">
+    <row r="39" spans="1:13" s="55" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="60" t="s">
         <v>341</v>
       </c>
@@ -6773,7 +6804,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="40" spans="1:13" s="38" customFormat="1" hidden="1">
+    <row r="40" spans="1:13" s="38" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="61"/>
       <c r="B40" s="35">
         <v>36</v>
@@ -6808,7 +6839,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="41" spans="1:13" s="55" customFormat="1">
+    <row r="41" spans="1:13" s="55" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="60" t="s">
         <v>341</v>
       </c>
@@ -6848,7 +6879,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="42" spans="1:13" s="42" customFormat="1" hidden="1">
+    <row r="42" spans="1:13" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="62"/>
       <c r="B42" s="39">
         <v>38</v>
@@ -6884,7 +6915,7 @@
       </c>
       <c r="M42" s="39"/>
     </row>
-    <row r="43" spans="1:13" s="71" customFormat="1">
+    <row r="43" spans="1:13" s="71" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="67" t="s">
         <v>341</v>
       </c>
@@ -6919,7 +6950,7 @@
       <c r="L43" s="70"/>
       <c r="M43" s="68"/>
     </row>
-    <row r="44" spans="1:13" s="38" customFormat="1" hidden="1">
+    <row r="44" spans="1:13" s="38" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="61"/>
       <c r="B44" s="35">
         <v>40</v>
@@ -6948,7 +6979,7 @@
       <c r="L44" s="37"/>
       <c r="M44" s="35"/>
     </row>
-    <row r="45" spans="1:13" s="55" customFormat="1">
+    <row r="45" spans="1:13" s="55" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="60" t="s">
         <v>341</v>
       </c>
@@ -6988,7 +7019,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="46" spans="1:13" s="38" customFormat="1" hidden="1">
+    <row r="46" spans="1:13" s="38" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="61"/>
       <c r="B46" s="35">
         <v>42</v>
@@ -7019,7 +7050,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="47" spans="1:13" s="50" customFormat="1" hidden="1">
+    <row r="47" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="63"/>
       <c r="B47" s="47">
         <v>43</v>
@@ -7052,7 +7083,7 @@
       <c r="L47" s="49"/>
       <c r="M47" s="47"/>
     </row>
-    <row r="48" spans="1:13" s="55" customFormat="1">
+    <row r="48" spans="1:13" s="55" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="60" t="s">
         <v>341</v>
       </c>
@@ -7087,7 +7118,7 @@
       <c r="L48" s="54"/>
       <c r="M48" s="51"/>
     </row>
-    <row r="49" spans="1:13" s="55" customFormat="1">
+    <row r="49" spans="1:13" s="55" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="60" t="s">
         <v>341</v>
       </c>
@@ -7122,7 +7153,7 @@
       <c r="L49" s="54"/>
       <c r="M49" s="51"/>
     </row>
-    <row r="50" spans="1:13" s="50" customFormat="1" hidden="1">
+    <row r="50" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="63"/>
       <c r="B50" s="47">
         <v>46</v>
@@ -7158,7 +7189,7 @@
       </c>
       <c r="M50" s="47"/>
     </row>
-    <row r="51" spans="1:13" s="55" customFormat="1">
+    <row r="51" spans="1:13" s="55" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="60" t="s">
         <v>341</v>
       </c>
@@ -7217,20 +7248,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.1640625" customWidth="1"/>
     <col min="5" max="5" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="60">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
@@ -7256,7 +7287,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1">
+    <row r="2" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -7290,7 +7321,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>288</v>
       </c>
@@ -7324,7 +7355,7 @@
         <v>1194</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>289</v>
       </c>
@@ -7358,7 +7389,7 @@
         <v>1393</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>287</v>
       </c>
@@ -7392,7 +7423,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>286</v>
       </c>
@@ -7426,7 +7457,7 @@
         <v>5174</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>285</v>
       </c>
@@ -7460,7 +7491,7 @@
         <v>5572</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>323</v>
       </c>
@@ -7494,7 +7525,7 @@
         <v>3184</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>1</v>
       </c>
@@ -7537,20 +7568,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:S22"/>
   <sheetViews>
     <sheetView showRuler="0" topLeftCell="G1" workbookViewId="0">
       <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="18.6640625" customWidth="1"/>
     <col min="7" max="7" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>105</v>
       </c>
@@ -7609,7 +7640,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>109</v>
       </c>
@@ -7659,7 +7690,7 @@
         <v>272.81</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>109</v>
       </c>
@@ -7712,7 +7743,7 @@
         <v>5300.38</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>109</v>
       </c>
@@ -7765,7 +7796,7 @@
         <v>7886.79</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>109</v>
       </c>
@@ -7818,7 +7849,7 @@
         <v>20060.93</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>109</v>
       </c>
@@ -7871,7 +7902,7 @@
         <v>3286.41</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>109</v>
       </c>
@@ -7924,7 +7955,7 @@
         <v>258.35000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>109</v>
       </c>
@@ -7977,7 +8008,7 @@
         <v>5207.08</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>109</v>
       </c>
@@ -8030,7 +8061,7 @@
         <v>7703.77</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>109</v>
       </c>
@@ -8083,7 +8114,7 @@
         <v>21166.34</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>109</v>
       </c>
@@ -8136,7 +8167,7 @@
         <v>3419.83</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="E12">
         <v>85.1</v>
       </c>
@@ -8159,7 +8190,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="E13">
         <v>135</v>
       </c>
@@ -8182,7 +8213,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="E14">
         <v>357</v>
       </c>
@@ -8205,7 +8236,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="E15">
         <v>58.6</v>
       </c>
@@ -8228,7 +8259,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
         <v>77</v>
       </c>
@@ -8236,7 +8267,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>106</v>
       </c>
@@ -8252,7 +8283,7 @@
         <v>101.99999999999997</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20">
         <v>6</v>
       </c>
@@ -8265,7 +8296,7 @@
         <v>659.40000000000009</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21">
         <v>7</v>
       </c>
@@ -8278,7 +8309,7 @@
         <v>243.60000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B22">
         <v>8</v>
       </c>
@@ -8303,14 +8334,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="C1" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="D1" workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="26.1640625" customWidth="1"/>
     <col min="4" max="4" width="16.83203125" customWidth="1"/>
@@ -8321,7 +8352,7 @@
     <col min="11" max="11" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" ht="28" customHeight="1">
+    <row r="1" spans="1:19" s="1" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>105</v>
       </c>
@@ -8380,7 +8411,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>81</v>
       </c>
@@ -8430,7 +8461,7 @@
         <v>15274.7</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -8480,7 +8511,7 @@
         <v>20155.96</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>123</v>
       </c>
@@ -8534,7 +8565,7 @@
         <v>14764.72</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>81</v>
       </c>
@@ -8584,7 +8615,7 @@
         <v>8615.4</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>81</v>
       </c>
@@ -8634,7 +8665,7 @@
         <v>21311.439999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>123</v>
       </c>
@@ -8688,7 +8719,7 @@
         <v>15461.96</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>81</v>
       </c>
@@ -8738,7 +8769,7 @@
         <v>17220.68</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>81</v>
       </c>
@@ -8788,7 +8819,7 @@
         <v>9633.73</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>81</v>
       </c>
@@ -8838,7 +8869,7 @@
         <v>18589.16</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -8892,7 +8923,7 @@
         <v>12880.36</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>81</v>
       </c>
@@ -8942,7 +8973,7 @@
         <v>7379.99</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="I14" t="s">
         <v>129</v>
       </c>
@@ -8950,7 +8981,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="I15" t="s">
         <v>130</v>
       </c>
@@ -8958,7 +8989,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="I16" t="s">
         <v>128</v>
       </c>
@@ -8968,7 +8999,7 @@
       </c>
       <c r="K16" s="6"/>
     </row>
-    <row r="17" spans="9:10">
+    <row r="17" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I17" t="s">
         <v>131</v>
       </c>
@@ -8976,7 +9007,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="9:10">
+    <row r="18" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I18" t="s">
         <v>132</v>
       </c>
@@ -8985,7 +9016,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="19" spans="9:10">
+    <row r="19" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I19" t="s">
         <v>133</v>
       </c>
@@ -9009,14 +9040,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:U25"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="19.1640625" customWidth="1"/>
     <col min="7" max="7" width="14.1640625" customWidth="1"/>
@@ -9024,7 +9055,7 @@
     <col min="11" max="11" width="13.6640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>105</v>
       </c>
@@ -9089,7 +9120,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>182</v>
       </c>
@@ -9150,7 +9181,7 @@
         <v>28118.33</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>182</v>
       </c>
@@ -9211,7 +9242,7 @@
         <v>29991.73</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>182</v>
       </c>
@@ -9272,7 +9303,7 @@
         <v>32013.200000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>182</v>
       </c>
@@ -9333,7 +9364,7 @@
         <v>32244.98</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>182</v>
       </c>
@@ -9394,7 +9425,7 @@
         <v>27377.31</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>182</v>
       </c>
@@ -9455,7 +9486,7 @@
         <v>32767.59</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>182</v>
       </c>
@@ -9516,7 +9547,7 @@
         <v>36563.31</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>182</v>
       </c>
@@ -9577,7 +9608,7 @@
         <v>35557.980000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>182</v>
       </c>
@@ -9638,7 +9669,7 @@
         <v>32475.17</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>182</v>
       </c>
@@ -9699,7 +9730,7 @@
         <v>37392.65</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>182</v>
       </c>
@@ -9760,7 +9791,7 @@
         <v>36902.019999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>182</v>
       </c>
@@ -9821,7 +9852,7 @@
         <v>37966.9</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>182</v>
       </c>
@@ -9883,7 +9914,7 @@
         <v>30055.55</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>182</v>
       </c>
@@ -9945,7 +9976,7 @@
         <v>30067.66</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>182</v>
       </c>
@@ -10007,7 +10038,7 @@
         <v>34401.22</v>
       </c>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>182</v>
       </c>
@@ -10069,7 +10100,7 @@
         <v>33439</v>
       </c>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>182</v>
       </c>
@@ -10130,7 +10161,7 @@
         <v>30110.560000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>182</v>
       </c>
@@ -10192,7 +10223,7 @@
         <v>31571.759999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>182</v>
       </c>
@@ -10254,7 +10285,7 @@
         <v>32668.43</v>
       </c>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>182</v>
       </c>
@@ -10315,7 +10346,7 @@
         <v>34665.15</v>
       </c>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>182</v>
       </c>
@@ -10377,7 +10408,7 @@
         <v>30294.65</v>
       </c>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>182</v>
       </c>
@@ -10439,7 +10470,7 @@
         <v>37081.919999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:20">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>182</v>
       </c>
@@ -10500,7 +10531,7 @@
         <v>29828.69</v>
       </c>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>182</v>
       </c>
@@ -10576,21 +10607,23 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:S27"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:J27"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.83203125" style="25" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" customWidth="1"/>
+    <col min="8" max="8" width="16.1640625" customWidth="1"/>
     <col min="10" max="10" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>105</v>
       </c>
@@ -10649,7 +10682,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>294</v>
       </c>
@@ -10703,7 +10736,7 @@
         <v>528.9</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>294</v>
       </c>
@@ -10757,7 +10790,7 @@
         <v>1784.48</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>294</v>
       </c>
@@ -10811,7 +10844,7 @@
         <v>1134.52</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>294</v>
       </c>
@@ -10865,7 +10898,7 @@
         <v>908.73</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>294</v>
       </c>
@@ -10919,7 +10952,7 @@
         <v>300.64999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>294</v>
       </c>
@@ -10973,7 +11006,7 @@
         <v>1356.94</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>294</v>
       </c>
@@ -11027,7 +11060,7 @@
         <v>549.6</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>294</v>
       </c>
@@ -11081,7 +11114,7 @@
         <v>698.67</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>294</v>
       </c>
@@ -11135,7 +11168,7 @@
         <v>1685.36</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>294</v>
       </c>
@@ -11189,7 +11222,7 @@
         <v>1266.1600000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>294</v>
       </c>
@@ -11243,7 +11276,7 @@
         <v>249.82</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>294</v>
       </c>
@@ -11297,7 +11330,7 @@
         <v>940.01</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>294</v>
       </c>
@@ -11351,7 +11384,7 @@
         <v>1244.8900000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>294</v>
       </c>
@@ -11405,7 +11438,7 @@
         <v>1375.75</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>294</v>
       </c>
@@ -11459,7 +11492,7 @@
         <v>583.87</v>
       </c>
     </row>
-    <row r="17" spans="1:19">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>294</v>
       </c>
@@ -11513,7 +11546,7 @@
         <v>550.66</v>
       </c>
     </row>
-    <row r="18" spans="1:19">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>294</v>
       </c>
@@ -11567,7 +11600,7 @@
         <v>1474.06</v>
       </c>
     </row>
-    <row r="19" spans="1:19">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>294</v>
       </c>
@@ -11621,7 +11654,7 @@
         <v>365.7</v>
       </c>
     </row>
-    <row r="20" spans="1:19">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>294</v>
       </c>
@@ -11675,7 +11708,7 @@
         <v>1184.97</v>
       </c>
     </row>
-    <row r="21" spans="1:19">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>294</v>
       </c>
@@ -11729,7 +11762,7 @@
         <v>803.93</v>
       </c>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>294</v>
       </c>
@@ -11783,7 +11816,7 @@
         <v>1196.44</v>
       </c>
     </row>
-    <row r="23" spans="1:19">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>294</v>
       </c>
@@ -11837,7 +11870,7 @@
         <v>957.01</v>
       </c>
     </row>
-    <row r="24" spans="1:19">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>294</v>
       </c>
@@ -11891,7 +11924,7 @@
         <v>1769.69</v>
       </c>
     </row>
-    <row r="25" spans="1:19">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>294</v>
       </c>
@@ -11945,7 +11978,7 @@
         <v>1576.65</v>
       </c>
     </row>
-    <row r="26" spans="1:19">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>294</v>
       </c>
@@ -11999,7 +12032,7 @@
         <v>2354.44</v>
       </c>
     </row>
-    <row r="27" spans="1:19">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>294</v>
       </c>
@@ -12068,21 +12101,21 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:R15"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G15"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="21.5" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
     <col min="7" max="7" width="23.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>105</v>
       </c>
@@ -12138,7 +12171,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>324</v>
       </c>
@@ -12188,7 +12221,7 @@
         <v>662.83</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>324</v>
       </c>
@@ -12238,7 +12271,7 @@
         <v>744.91</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>324</v>
       </c>
@@ -12288,7 +12321,7 @@
         <v>72.5</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>324</v>
       </c>
@@ -12338,7 +12371,7 @@
         <v>1108.97</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>324</v>
       </c>
@@ -12388,7 +12421,7 @@
         <v>141.08000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>324</v>
       </c>
@@ -12438,7 +12471,7 @@
         <v>1672.84</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>324</v>
       </c>
@@ -12488,7 +12521,7 @@
         <v>80.62</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>324</v>
       </c>
@@ -12538,7 +12571,7 @@
         <v>756.12</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>324</v>
       </c>
@@ -12588,7 +12621,7 @@
         <v>37.49</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>324</v>
       </c>
@@ -12638,7 +12671,7 @@
         <v>1803.22</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>324</v>
       </c>
@@ -12688,7 +12721,7 @@
         <v>1843.26</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>324</v>
       </c>
@@ -12738,7 +12771,7 @@
         <v>1689.42</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>324</v>
       </c>
@@ -12788,7 +12821,7 @@
         <v>883.76</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>324</v>
       </c>
@@ -12853,17 +12886,17 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P33"/>
+  <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.5" style="181" customWidth="1"/>
     <col min="2" max="2" width="13" style="181" customWidth="1"/>
@@ -12872,17 +12905,18 @@
     <col min="5" max="5" width="12.5" style="182" customWidth="1"/>
     <col min="6" max="6" width="10.83203125" style="182" customWidth="1"/>
     <col min="7" max="7" width="10.83203125" style="183" customWidth="1"/>
-    <col min="8" max="8" width="21.5" style="182" customWidth="1"/>
-    <col min="9" max="9" width="12.1640625" style="182" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" style="182" customWidth="1"/>
-    <col min="11" max="11" width="24" style="184" customWidth="1"/>
-    <col min="12" max="12" width="24.33203125" style="185" customWidth="1"/>
-    <col min="13" max="13" width="89.83203125" style="182" customWidth="1"/>
-    <col min="14" max="14" width="31.83203125" style="182" customWidth="1"/>
-    <col min="15" max="16384" width="10.83203125" style="182"/>
+    <col min="8" max="8" width="14.33203125" style="183" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.5" style="182" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" style="182" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" style="182" customWidth="1"/>
+    <col min="12" max="12" width="24" style="184" customWidth="1"/>
+    <col min="13" max="13" width="24.33203125" style="185" customWidth="1"/>
+    <col min="14" max="14" width="89.83203125" style="182" customWidth="1"/>
+    <col min="15" max="15" width="31.83203125" style="182" customWidth="1"/>
+    <col min="16" max="16384" width="10.83203125" style="182"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="132" customFormat="1" ht="42" customHeight="1">
+    <row r="1" spans="1:17" s="132" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="128" t="s">
         <v>342</v>
       </c>
@@ -12905,28 +12939,31 @@
         <v>355</v>
       </c>
       <c r="H1" s="128" t="s">
+        <v>362</v>
+      </c>
+      <c r="I1" s="128" t="s">
         <v>177</v>
       </c>
-      <c r="I1" s="128" t="s">
+      <c r="J1" s="128" t="s">
         <v>356</v>
       </c>
-      <c r="J1" s="128" t="s">
+      <c r="K1" s="128" t="s">
         <v>357</v>
       </c>
-      <c r="K1" s="130" t="s">
+      <c r="L1" s="130" t="s">
         <v>321</v>
       </c>
-      <c r="L1" s="131" t="s">
+      <c r="M1" s="131" t="s">
         <v>322</v>
       </c>
-      <c r="M1" s="128" t="s">
+      <c r="N1" s="128" t="s">
         <v>274</v>
       </c>
-      <c r="N1" s="65" t="s">
+      <c r="O1" s="65" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="140" customFormat="1">
+    <row r="2" spans="1:17" s="140" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="133">
         <v>1</v>
       </c>
@@ -12948,27 +12985,30 @@
       <c r="G2" s="135">
         <v>2</v>
       </c>
-      <c r="H2" s="134" t="s">
+      <c r="H2" s="135" t="s">
+        <v>363</v>
+      </c>
+      <c r="I2" s="134" t="s">
         <v>261</v>
       </c>
-      <c r="I2" s="136">
+      <c r="J2" s="136">
         <v>42833</v>
       </c>
-      <c r="J2" s="136">
+      <c r="K2" s="136">
         <v>43186</v>
       </c>
-      <c r="K2" s="137">
+      <c r="L2" s="137">
         <v>84</v>
       </c>
-      <c r="L2" s="138">
-        <f t="shared" ref="L2:L13" si="0">K2*46</f>
+      <c r="M2" s="138">
+        <f t="shared" ref="M2:M13" si="0">L2*46</f>
         <v>3864</v>
       </c>
-      <c r="M2" s="134"/>
-      <c r="N2" s="139"/>
-      <c r="P2" s="139"/>
-    </row>
-    <row r="3" spans="1:16" s="140" customFormat="1">
+      <c r="N2" s="134"/>
+      <c r="O2" s="139"/>
+      <c r="Q2" s="139"/>
+    </row>
+    <row r="3" spans="1:17" s="140" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="133">
         <v>1</v>
       </c>
@@ -12990,27 +13030,30 @@
       <c r="G3" s="135">
         <v>2</v>
       </c>
-      <c r="H3" s="134" t="s">
+      <c r="H3" s="135" t="s">
+        <v>363</v>
+      </c>
+      <c r="I3" s="134" t="s">
         <v>261</v>
       </c>
-      <c r="I3" s="136">
+      <c r="J3" s="136">
         <v>42833</v>
       </c>
-      <c r="J3" s="136">
+      <c r="K3" s="136">
         <v>43186</v>
       </c>
-      <c r="K3" s="137">
+      <c r="L3" s="137">
         <v>43.9</v>
       </c>
-      <c r="L3" s="138">
+      <c r="M3" s="138">
         <f t="shared" si="0"/>
         <v>2019.3999999999999</v>
       </c>
-      <c r="M3" s="134"/>
-      <c r="N3" s="139"/>
-      <c r="P3" s="139"/>
-    </row>
-    <row r="4" spans="1:16" s="140" customFormat="1">
+      <c r="N3" s="134"/>
+      <c r="O3" s="139"/>
+      <c r="Q3" s="139"/>
+    </row>
+    <row r="4" spans="1:17" s="140" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="133">
         <v>1</v>
       </c>
@@ -13032,27 +13075,30 @@
       <c r="G4" s="135">
         <v>2</v>
       </c>
-      <c r="H4" s="134" t="s">
+      <c r="H4" s="135" t="s">
+        <v>363</v>
+      </c>
+      <c r="I4" s="134" t="s">
         <v>261</v>
       </c>
-      <c r="I4" s="136">
+      <c r="J4" s="136">
         <v>42833</v>
       </c>
-      <c r="J4" s="136">
+      <c r="K4" s="136">
         <v>43186</v>
       </c>
-      <c r="K4" s="137">
+      <c r="L4" s="137">
         <v>56</v>
       </c>
-      <c r="L4" s="138">
+      <c r="M4" s="138">
         <f t="shared" si="0"/>
         <v>2576</v>
       </c>
-      <c r="M4" s="134"/>
-      <c r="N4" s="139"/>
-      <c r="P4" s="139"/>
-    </row>
-    <row r="5" spans="1:16" s="140" customFormat="1">
+      <c r="N4" s="134"/>
+      <c r="O4" s="139"/>
+      <c r="Q4" s="139"/>
+    </row>
+    <row r="5" spans="1:17" s="140" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="133">
         <v>2</v>
       </c>
@@ -13074,27 +13120,30 @@
       <c r="G5" s="135">
         <v>2</v>
       </c>
-      <c r="H5" s="134" t="s">
+      <c r="H5" s="135" t="s">
+        <v>363</v>
+      </c>
+      <c r="I5" s="134" t="s">
         <v>261</v>
       </c>
-      <c r="I5" s="136">
+      <c r="J5" s="136">
         <v>42833</v>
       </c>
-      <c r="J5" s="136">
+      <c r="K5" s="136">
         <v>43186</v>
       </c>
-      <c r="K5" s="137">
+      <c r="L5" s="137">
         <v>24.2</v>
       </c>
-      <c r="L5" s="138">
+      <c r="M5" s="138">
         <f t="shared" si="0"/>
         <v>1113.2</v>
       </c>
-      <c r="M5" s="134"/>
-      <c r="N5" s="139"/>
-      <c r="P5" s="139"/>
-    </row>
-    <row r="6" spans="1:16" s="140" customFormat="1">
+      <c r="N5" s="134"/>
+      <c r="O5" s="139"/>
+      <c r="Q5" s="139"/>
+    </row>
+    <row r="6" spans="1:17" s="140" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="133">
         <v>3</v>
       </c>
@@ -13116,27 +13165,30 @@
       <c r="G6" s="135">
         <v>0</v>
       </c>
-      <c r="H6" s="134" t="s">
+      <c r="H6" s="135" t="s">
+        <v>363</v>
+      </c>
+      <c r="I6" s="134" t="s">
         <v>261</v>
       </c>
-      <c r="I6" s="136">
+      <c r="J6" s="136">
         <v>42833</v>
       </c>
-      <c r="J6" s="136">
+      <c r="K6" s="136">
         <v>43186</v>
       </c>
-      <c r="K6" s="137">
+      <c r="L6" s="137">
         <v>33.200000000000003</v>
       </c>
-      <c r="L6" s="138">
+      <c r="M6" s="138">
         <f t="shared" si="0"/>
         <v>1527.2</v>
       </c>
-      <c r="M6" s="134"/>
-      <c r="N6" s="139"/>
-      <c r="P6" s="139"/>
-    </row>
-    <row r="7" spans="1:16" s="148" customFormat="1">
+      <c r="N6" s="134"/>
+      <c r="O6" s="139"/>
+      <c r="Q6" s="139"/>
+    </row>
+    <row r="7" spans="1:17" s="148" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="141">
         <v>1</v>
       </c>
@@ -13158,27 +13210,30 @@
       <c r="G7" s="143">
         <v>2</v>
       </c>
-      <c r="H7" s="142" t="s">
+      <c r="H7" s="143" t="s">
+        <v>363</v>
+      </c>
+      <c r="I7" s="142" t="s">
         <v>261</v>
       </c>
-      <c r="I7" s="144">
+      <c r="J7" s="144">
         <v>42833</v>
       </c>
-      <c r="J7" s="144">
+      <c r="K7" s="144">
         <v>43186</v>
       </c>
-      <c r="K7" s="145">
+      <c r="L7" s="145">
         <v>76</v>
       </c>
-      <c r="L7" s="146">
+      <c r="M7" s="146">
         <f t="shared" si="0"/>
         <v>3496</v>
       </c>
-      <c r="M7" s="142"/>
-      <c r="N7" s="147"/>
-      <c r="P7" s="147"/>
-    </row>
-    <row r="8" spans="1:16" s="148" customFormat="1">
+      <c r="N7" s="142"/>
+      <c r="O7" s="147"/>
+      <c r="Q7" s="147"/>
+    </row>
+    <row r="8" spans="1:17" s="148" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="141">
         <v>1</v>
       </c>
@@ -13200,27 +13255,30 @@
       <c r="G8" s="143">
         <v>2</v>
       </c>
-      <c r="H8" s="142" t="s">
+      <c r="H8" s="143" t="s">
+        <v>363</v>
+      </c>
+      <c r="I8" s="142" t="s">
         <v>261</v>
       </c>
-      <c r="I8" s="144">
+      <c r="J8" s="144">
         <v>42833</v>
       </c>
-      <c r="J8" s="144">
+      <c r="K8" s="144">
         <v>43186</v>
       </c>
-      <c r="K8" s="145">
+      <c r="L8" s="145">
         <v>51</v>
       </c>
-      <c r="L8" s="146">
+      <c r="M8" s="146">
         <f t="shared" si="0"/>
         <v>2346</v>
       </c>
-      <c r="M8" s="142"/>
-      <c r="N8" s="147"/>
-      <c r="P8" s="147"/>
-    </row>
-    <row r="9" spans="1:16" s="148" customFormat="1">
+      <c r="N8" s="142"/>
+      <c r="O8" s="147"/>
+      <c r="Q8" s="147"/>
+    </row>
+    <row r="9" spans="1:17" s="148" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="141">
         <v>1</v>
       </c>
@@ -13242,27 +13300,30 @@
       <c r="G9" s="143">
         <v>2</v>
       </c>
-      <c r="H9" s="142" t="s">
+      <c r="H9" s="143" t="s">
+        <v>363</v>
+      </c>
+      <c r="I9" s="142" t="s">
         <v>261</v>
       </c>
-      <c r="I9" s="144">
+      <c r="J9" s="144">
         <v>42833</v>
       </c>
-      <c r="J9" s="144">
+      <c r="K9" s="144">
         <v>43186</v>
       </c>
-      <c r="K9" s="145">
+      <c r="L9" s="145">
         <v>34.6</v>
       </c>
-      <c r="L9" s="146">
+      <c r="M9" s="146">
         <f t="shared" si="0"/>
         <v>1591.6000000000001</v>
       </c>
-      <c r="M9" s="142"/>
-      <c r="N9" s="147"/>
-      <c r="P9" s="147"/>
-    </row>
-    <row r="10" spans="1:16" s="148" customFormat="1">
+      <c r="N9" s="142"/>
+      <c r="O9" s="147"/>
+      <c r="Q9" s="147"/>
+    </row>
+    <row r="10" spans="1:17" s="148" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="141">
         <v>1</v>
       </c>
@@ -13284,27 +13345,30 @@
       <c r="G10" s="143">
         <v>3</v>
       </c>
-      <c r="H10" s="142" t="s">
+      <c r="H10" s="143" t="s">
+        <v>363</v>
+      </c>
+      <c r="I10" s="142" t="s">
         <v>261</v>
       </c>
-      <c r="I10" s="144">
+      <c r="J10" s="144">
         <v>42833</v>
       </c>
-      <c r="J10" s="144">
+      <c r="K10" s="144">
         <v>43186</v>
       </c>
-      <c r="K10" s="145">
+      <c r="L10" s="145">
         <v>49.6</v>
       </c>
-      <c r="L10" s="146">
+      <c r="M10" s="146">
         <f t="shared" si="0"/>
         <v>2281.6</v>
       </c>
-      <c r="M10" s="142"/>
-      <c r="N10" s="147"/>
-      <c r="P10" s="147"/>
-    </row>
-    <row r="11" spans="1:16" s="148" customFormat="1">
+      <c r="N10" s="142"/>
+      <c r="O10" s="147"/>
+      <c r="Q10" s="147"/>
+    </row>
+    <row r="11" spans="1:17" s="148" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="141">
         <v>1</v>
       </c>
@@ -13326,27 +13390,30 @@
       <c r="G11" s="143">
         <v>3</v>
       </c>
-      <c r="H11" s="142" t="s">
+      <c r="H11" s="143" t="s">
+        <v>363</v>
+      </c>
+      <c r="I11" s="142" t="s">
         <v>261</v>
       </c>
-      <c r="I11" s="144">
+      <c r="J11" s="144">
         <v>42833</v>
       </c>
-      <c r="J11" s="144">
+      <c r="K11" s="144">
         <v>43186</v>
       </c>
-      <c r="K11" s="145">
+      <c r="L11" s="145">
         <v>57</v>
       </c>
-      <c r="L11" s="146">
+      <c r="M11" s="146">
         <f t="shared" si="0"/>
         <v>2622</v>
       </c>
-      <c r="M11" s="142"/>
-      <c r="N11" s="147"/>
-      <c r="P11" s="147"/>
-    </row>
-    <row r="12" spans="1:16" s="148" customFormat="1">
+      <c r="N11" s="142"/>
+      <c r="O11" s="147"/>
+      <c r="Q11" s="147"/>
+    </row>
+    <row r="12" spans="1:17" s="148" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="141">
         <v>2</v>
       </c>
@@ -13368,27 +13435,30 @@
       <c r="G12" s="143">
         <v>2</v>
       </c>
-      <c r="H12" s="142" t="s">
+      <c r="H12" s="143" t="s">
+        <v>363</v>
+      </c>
+      <c r="I12" s="142" t="s">
         <v>261</v>
       </c>
-      <c r="I12" s="144">
+      <c r="J12" s="144">
         <v>42833</v>
       </c>
-      <c r="J12" s="144">
+      <c r="K12" s="144">
         <v>43186</v>
       </c>
-      <c r="K12" s="145">
+      <c r="L12" s="145">
         <v>18.3</v>
       </c>
-      <c r="L12" s="146">
+      <c r="M12" s="146">
         <f t="shared" si="0"/>
         <v>841.80000000000007</v>
       </c>
-      <c r="M12" s="142"/>
-      <c r="N12" s="147"/>
-      <c r="P12" s="147"/>
-    </row>
-    <row r="13" spans="1:16" s="148" customFormat="1">
+      <c r="N12" s="142"/>
+      <c r="O12" s="147"/>
+      <c r="Q12" s="147"/>
+    </row>
+    <row r="13" spans="1:17" s="148" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="141">
         <v>3</v>
       </c>
@@ -13410,27 +13480,30 @@
       <c r="G13" s="143">
         <v>2</v>
       </c>
-      <c r="H13" s="142" t="s">
+      <c r="H13" s="143" t="s">
+        <v>363</v>
+      </c>
+      <c r="I13" s="142" t="s">
         <v>261</v>
       </c>
-      <c r="I13" s="144">
+      <c r="J13" s="144">
         <v>42833</v>
       </c>
-      <c r="J13" s="144">
+      <c r="K13" s="144">
         <v>43186</v>
       </c>
-      <c r="K13" s="145">
+      <c r="L13" s="145">
         <v>19.600000000000001</v>
       </c>
-      <c r="L13" s="146">
+      <c r="M13" s="146">
         <f t="shared" si="0"/>
         <v>901.6</v>
       </c>
-      <c r="M13" s="142"/>
-      <c r="N13" s="147"/>
-      <c r="P13" s="147"/>
-    </row>
-    <row r="14" spans="1:16" s="30" customFormat="1">
+      <c r="N13" s="142"/>
+      <c r="O13" s="147"/>
+      <c r="Q13" s="147"/>
+    </row>
+    <row r="14" spans="1:17" s="30" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="124">
         <v>1</v>
       </c>
@@ -13452,26 +13525,29 @@
       <c r="G14" s="122">
         <v>3</v>
       </c>
-      <c r="H14" s="27" t="s">
+      <c r="H14" s="122" t="s">
+        <v>363</v>
+      </c>
+      <c r="I14" s="27" t="s">
         <v>261</v>
       </c>
-      <c r="I14" s="32">
+      <c r="J14" s="32">
         <v>42833</v>
       </c>
-      <c r="J14" s="32" t="s">
+      <c r="K14" s="32" t="s">
         <v>358</v>
       </c>
-      <c r="K14" s="58" t="s">
+      <c r="L14" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="L14" s="108" t="s">
+      <c r="M14" s="108" t="s">
         <v>74</v>
       </c>
-      <c r="M14" s="27"/>
-      <c r="N14" s="34"/>
-      <c r="P14" s="34"/>
-    </row>
-    <row r="15" spans="1:16" s="156" customFormat="1">
+      <c r="N14" s="27"/>
+      <c r="O14" s="34"/>
+      <c r="Q14" s="34"/>
+    </row>
+    <row r="15" spans="1:17" s="156" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="149">
         <v>1</v>
       </c>
@@ -13493,27 +13569,30 @@
       <c r="G15" s="151">
         <v>2</v>
       </c>
-      <c r="H15" s="150" t="s">
+      <c r="H15" s="151" t="s">
+        <v>363</v>
+      </c>
+      <c r="I15" s="150" t="s">
         <v>261</v>
       </c>
-      <c r="I15" s="152">
+      <c r="J15" s="152">
         <v>42833</v>
       </c>
-      <c r="J15" s="152">
+      <c r="K15" s="152">
         <v>43186</v>
       </c>
-      <c r="K15" s="153">
+      <c r="L15" s="153">
         <v>63</v>
       </c>
-      <c r="L15" s="154">
-        <f>K15*46</f>
+      <c r="M15" s="154">
+        <f>L15*46</f>
         <v>2898</v>
       </c>
-      <c r="M15" s="150"/>
-      <c r="N15" s="155"/>
-      <c r="P15" s="155"/>
-    </row>
-    <row r="16" spans="1:16" s="156" customFormat="1">
+      <c r="N15" s="150"/>
+      <c r="O15" s="155"/>
+      <c r="Q15" s="155"/>
+    </row>
+    <row r="16" spans="1:17" s="156" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="149">
         <v>1</v>
       </c>
@@ -13535,27 +13614,30 @@
       <c r="G16" s="151">
         <v>2</v>
       </c>
-      <c r="H16" s="150" t="s">
+      <c r="H16" s="151" t="s">
+        <v>363</v>
+      </c>
+      <c r="I16" s="150" t="s">
         <v>261</v>
       </c>
-      <c r="I16" s="152">
+      <c r="J16" s="152">
         <v>42833</v>
       </c>
-      <c r="J16" s="152">
+      <c r="K16" s="152">
         <v>43186</v>
       </c>
-      <c r="K16" s="153">
+      <c r="L16" s="153">
         <v>46.5</v>
       </c>
-      <c r="L16" s="154">
-        <f>K16*46</f>
+      <c r="M16" s="154">
+        <f>L16*46</f>
         <v>2139</v>
       </c>
-      <c r="M16" s="150"/>
-      <c r="N16" s="155"/>
-      <c r="P16" s="155"/>
-    </row>
-    <row r="17" spans="1:16" s="156" customFormat="1">
+      <c r="N16" s="150"/>
+      <c r="O16" s="155"/>
+      <c r="Q16" s="155"/>
+    </row>
+    <row r="17" spans="1:17" s="156" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="149">
         <v>1</v>
       </c>
@@ -13577,27 +13659,30 @@
       <c r="G17" s="151">
         <v>2</v>
       </c>
-      <c r="H17" s="150" t="s">
+      <c r="H17" s="151" t="s">
+        <v>363</v>
+      </c>
+      <c r="I17" s="150" t="s">
         <v>261</v>
       </c>
-      <c r="I17" s="152">
+      <c r="J17" s="152">
         <v>42833</v>
       </c>
-      <c r="J17" s="152">
+      <c r="K17" s="152">
         <v>43186</v>
       </c>
-      <c r="K17" s="153">
+      <c r="L17" s="153">
         <v>28.6</v>
       </c>
-      <c r="L17" s="154">
-        <f>K17*46</f>
+      <c r="M17" s="154">
+        <f>L17*46</f>
         <v>1315.6000000000001</v>
       </c>
-      <c r="M17" s="150"/>
-      <c r="N17" s="155"/>
-      <c r="P17" s="155"/>
-    </row>
-    <row r="18" spans="1:16" s="156" customFormat="1">
+      <c r="N17" s="150"/>
+      <c r="O17" s="155"/>
+      <c r="Q17" s="155"/>
+    </row>
+    <row r="18" spans="1:17" s="156" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="149">
         <v>1</v>
       </c>
@@ -13619,27 +13704,30 @@
       <c r="G18" s="151">
         <v>2</v>
       </c>
-      <c r="H18" s="150" t="s">
+      <c r="H18" s="151" t="s">
+        <v>363</v>
+      </c>
+      <c r="I18" s="150" t="s">
         <v>261</v>
       </c>
-      <c r="I18" s="152">
+      <c r="J18" s="152">
         <v>42833</v>
       </c>
-      <c r="J18" s="152">
+      <c r="K18" s="152">
         <v>43186</v>
       </c>
-      <c r="K18" s="153">
+      <c r="L18" s="153">
         <v>47</v>
       </c>
-      <c r="L18" s="154">
-        <f>K18*46</f>
+      <c r="M18" s="154">
+        <f>L18*46</f>
         <v>2162</v>
       </c>
-      <c r="M18" s="150"/>
-      <c r="N18" s="155"/>
-      <c r="P18" s="155"/>
-    </row>
-    <row r="19" spans="1:16" s="156" customFormat="1">
+      <c r="N18" s="150"/>
+      <c r="O18" s="155"/>
+      <c r="Q18" s="155"/>
+    </row>
+    <row r="19" spans="1:17" s="156" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="149">
         <v>2</v>
       </c>
@@ -13661,26 +13749,29 @@
       <c r="G19" s="151">
         <v>2</v>
       </c>
-      <c r="H19" s="150" t="s">
+      <c r="H19" s="151" t="s">
+        <v>363</v>
+      </c>
+      <c r="I19" s="150" t="s">
         <v>261</v>
       </c>
-      <c r="I19" s="152">
+      <c r="J19" s="152">
         <v>42833</v>
       </c>
-      <c r="J19" s="152" t="s">
+      <c r="K19" s="152" t="s">
         <v>358</v>
       </c>
-      <c r="K19" s="153" t="s">
+      <c r="L19" s="153" t="s">
         <v>74</v>
       </c>
-      <c r="L19" s="154" t="s">
+      <c r="M19" s="154" t="s">
         <v>74</v>
       </c>
-      <c r="M19" s="150"/>
-      <c r="N19" s="155"/>
-      <c r="P19" s="155"/>
-    </row>
-    <row r="20" spans="1:16" s="156" customFormat="1">
+      <c r="N19" s="150"/>
+      <c r="O19" s="155"/>
+      <c r="Q19" s="155"/>
+    </row>
+    <row r="20" spans="1:17" s="156" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="149">
         <v>3</v>
       </c>
@@ -13702,26 +13793,29 @@
       <c r="G20" s="151">
         <v>3</v>
       </c>
-      <c r="H20" s="150" t="s">
+      <c r="H20" s="151" t="s">
+        <v>363</v>
+      </c>
+      <c r="I20" s="150" t="s">
         <v>261</v>
       </c>
-      <c r="I20" s="152">
+      <c r="J20" s="152">
         <v>42833</v>
       </c>
-      <c r="J20" s="152" t="s">
+      <c r="K20" s="152" t="s">
         <v>358</v>
       </c>
-      <c r="K20" s="153" t="s">
+      <c r="L20" s="153" t="s">
         <v>74</v>
       </c>
-      <c r="L20" s="154" t="s">
+      <c r="M20" s="154" t="s">
         <v>74</v>
       </c>
-      <c r="M20" s="150"/>
-      <c r="N20" s="155"/>
-      <c r="P20" s="155"/>
-    </row>
-    <row r="21" spans="1:16" s="115" customFormat="1">
+      <c r="N20" s="150"/>
+      <c r="O20" s="155"/>
+      <c r="Q20" s="155"/>
+    </row>
+    <row r="21" spans="1:17" s="115" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="125">
         <v>1</v>
       </c>
@@ -13743,25 +13837,28 @@
       <c r="G21" s="112">
         <v>2</v>
       </c>
-      <c r="H21" s="111" t="s">
+      <c r="H21" s="112" t="s">
+        <v>363</v>
+      </c>
+      <c r="I21" s="111" t="s">
         <v>261</v>
       </c>
-      <c r="I21" s="113">
+      <c r="J21" s="113">
         <v>42833</v>
       </c>
-      <c r="J21" s="113">
+      <c r="K21" s="113">
         <v>43186</v>
       </c>
-      <c r="K21" s="116">
+      <c r="L21" s="116">
         <v>69</v>
       </c>
-      <c r="L21" s="117">
-        <f>K21*46</f>
+      <c r="M21" s="117">
+        <f>L21*46</f>
         <v>3174</v>
       </c>
-      <c r="M21" s="111"/>
-    </row>
-    <row r="22" spans="1:16" s="115" customFormat="1">
+      <c r="N21" s="111"/>
+    </row>
+    <row r="22" spans="1:17" s="115" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="125">
         <v>1</v>
       </c>
@@ -13783,24 +13880,27 @@
       <c r="G22" s="112">
         <v>2</v>
       </c>
-      <c r="H22" s="111" t="s">
+      <c r="H22" s="112" t="s">
+        <v>363</v>
+      </c>
+      <c r="I22" s="111" t="s">
         <v>261</v>
       </c>
-      <c r="I22" s="113">
+      <c r="J22" s="113">
         <v>42833</v>
       </c>
-      <c r="J22" s="113">
+      <c r="K22" s="113">
         <v>43186</v>
       </c>
-      <c r="K22" s="116" t="s">
+      <c r="L22" s="116" t="s">
         <v>340</v>
       </c>
-      <c r="L22" s="117" t="s">
+      <c r="M22" s="117" t="s">
         <v>74</v>
       </c>
-      <c r="M22" s="111"/>
-    </row>
-    <row r="23" spans="1:16" s="115" customFormat="1">
+      <c r="N22" s="111"/>
+    </row>
+    <row r="23" spans="1:17" s="115" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="125">
         <v>1</v>
       </c>
@@ -13822,25 +13922,28 @@
       <c r="G23" s="112">
         <v>2</v>
       </c>
-      <c r="H23" s="111" t="s">
+      <c r="H23" s="112" t="s">
+        <v>363</v>
+      </c>
+      <c r="I23" s="111" t="s">
         <v>261</v>
       </c>
-      <c r="I23" s="113">
+      <c r="J23" s="113">
         <v>42833</v>
       </c>
-      <c r="J23" s="113">
+      <c r="K23" s="113">
         <v>43186</v>
       </c>
-      <c r="K23" s="116">
+      <c r="L23" s="116">
         <v>47.6</v>
       </c>
-      <c r="L23" s="117">
-        <f>K23*46</f>
+      <c r="M23" s="117">
+        <f>L23*46</f>
         <v>2189.6</v>
       </c>
-      <c r="M23" s="111"/>
-    </row>
-    <row r="24" spans="1:16" s="115" customFormat="1">
+      <c r="N23" s="111"/>
+    </row>
+    <row r="24" spans="1:17" s="115" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="125">
         <v>2</v>
       </c>
@@ -13862,22 +13965,25 @@
       <c r="G24" s="112">
         <v>3</v>
       </c>
-      <c r="H24" s="111" t="s">
+      <c r="H24" s="112" t="s">
+        <v>363</v>
+      </c>
+      <c r="I24" s="111" t="s">
         <v>261</v>
       </c>
-      <c r="I24" s="113">
+      <c r="J24" s="113">
         <v>42833</v>
       </c>
-      <c r="J24" s="113" t="s">
+      <c r="K24" s="113" t="s">
         <v>358</v>
       </c>
-      <c r="K24" s="109" t="s">
+      <c r="L24" s="109" t="s">
         <v>74</v>
       </c>
-      <c r="L24" s="117"/>
-      <c r="M24" s="111"/>
-    </row>
-    <row r="25" spans="1:16" s="115" customFormat="1">
+      <c r="M24" s="117"/>
+      <c r="N24" s="111"/>
+    </row>
+    <row r="25" spans="1:17" s="115" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="125">
         <v>3</v>
       </c>
@@ -13899,27 +14005,30 @@
       <c r="G25" s="112">
         <v>3</v>
       </c>
-      <c r="H25" s="111" t="s">
+      <c r="H25" s="112" t="s">
+        <v>363</v>
+      </c>
+      <c r="I25" s="111" t="s">
         <v>261</v>
       </c>
-      <c r="I25" s="113">
+      <c r="J25" s="113">
         <v>42833</v>
       </c>
-      <c r="J25" s="113">
+      <c r="K25" s="113">
         <v>43186</v>
       </c>
-      <c r="K25" s="116">
+      <c r="L25" s="116">
         <v>83</v>
       </c>
-      <c r="L25" s="117">
-        <f>K25*46</f>
+      <c r="M25" s="117">
+        <f>L25*46</f>
         <v>3818</v>
       </c>
-      <c r="M25" s="111"/>
-      <c r="N25" s="114"/>
-      <c r="P25" s="114"/>
-    </row>
-    <row r="26" spans="1:16" s="166" customFormat="1">
+      <c r="N25" s="111"/>
+      <c r="O25" s="114"/>
+      <c r="Q25" s="114"/>
+    </row>
+    <row r="26" spans="1:17" s="166" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="158">
         <v>1</v>
       </c>
@@ -13941,27 +14050,30 @@
       <c r="G26" s="162" t="s">
         <v>40</v>
       </c>
-      <c r="H26" s="161" t="s">
+      <c r="H26" s="162" t="s">
+        <v>352</v>
+      </c>
+      <c r="I26" s="161" t="s">
         <v>279</v>
       </c>
-      <c r="I26" s="163">
+      <c r="J26" s="163">
         <v>42905</v>
       </c>
-      <c r="J26" s="163">
+      <c r="K26" s="163">
         <v>43189</v>
       </c>
-      <c r="K26" s="164">
+      <c r="L26" s="164">
         <v>61.2</v>
       </c>
-      <c r="L26" s="165">
-        <f>K26*(20-1)</f>
+      <c r="M26" s="165">
+        <f>L26*(20-1)</f>
         <v>1162.8</v>
       </c>
-      <c r="M26" s="161" t="s">
+      <c r="N26" s="161" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="27" spans="1:16" s="166" customFormat="1">
+    <row r="27" spans="1:17" s="166" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="158">
         <v>1</v>
       </c>
@@ -13983,27 +14095,30 @@
       <c r="G27" s="162" t="s">
         <v>40</v>
       </c>
-      <c r="H27" s="161" t="s">
+      <c r="H27" s="162" t="s">
+        <v>349</v>
+      </c>
+      <c r="I27" s="161" t="s">
         <v>279</v>
       </c>
-      <c r="I27" s="163">
+      <c r="J27" s="163">
         <v>42878</v>
       </c>
-      <c r="J27" s="163">
+      <c r="K27" s="163">
         <v>43189</v>
       </c>
-      <c r="K27" s="164">
+      <c r="L27" s="164">
         <v>71</v>
       </c>
-      <c r="L27" s="165">
-        <f>K27*(20-1)</f>
+      <c r="M27" s="165">
+        <f>L27*(20-1)</f>
         <v>1349</v>
       </c>
-      <c r="M27" s="161" t="s">
+      <c r="N27" s="161" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="28" spans="1:16" s="166" customFormat="1">
+    <row r="28" spans="1:17" s="166" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="158">
         <v>1</v>
       </c>
@@ -14025,27 +14140,30 @@
       <c r="G28" s="162" t="s">
         <v>40</v>
       </c>
-      <c r="H28" s="161" t="s">
+      <c r="H28" s="162" t="s">
+        <v>349</v>
+      </c>
+      <c r="I28" s="161" t="s">
         <v>279</v>
       </c>
-      <c r="I28" s="163">
+      <c r="J28" s="163">
         <v>42901</v>
       </c>
-      <c r="J28" s="163">
+      <c r="K28" s="163">
         <v>43189</v>
       </c>
-      <c r="K28" s="164">
+      <c r="L28" s="164">
         <v>122</v>
       </c>
-      <c r="L28" s="165">
-        <f>K28*(20-1)</f>
+      <c r="M28" s="165">
+        <f>L28*(20-1)</f>
         <v>2318</v>
       </c>
-      <c r="M28" s="161" t="s">
+      <c r="N28" s="161" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="29" spans="1:16" s="172" customFormat="1">
+    <row r="29" spans="1:17" s="172" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="167">
         <v>1</v>
       </c>
@@ -14067,24 +14185,27 @@
       <c r="G29" s="162" t="s">
         <v>40</v>
       </c>
-      <c r="H29" s="168" t="s">
+      <c r="H29" s="162" t="s">
+        <v>349</v>
+      </c>
+      <c r="I29" s="168" t="s">
         <v>279</v>
       </c>
-      <c r="I29" s="169">
+      <c r="J29" s="169">
         <v>42892</v>
       </c>
-      <c r="J29" s="169">
+      <c r="K29" s="169">
         <v>43189</v>
       </c>
-      <c r="K29" s="170" t="s">
+      <c r="L29" s="170" t="s">
         <v>340</v>
       </c>
-      <c r="L29" s="171" t="s">
+      <c r="M29" s="171" t="s">
         <v>74</v>
       </c>
-      <c r="M29" s="168"/>
-    </row>
-    <row r="30" spans="1:16" s="180" customFormat="1">
+      <c r="N29" s="168"/>
+    </row>
+    <row r="30" spans="1:17" s="180" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="173">
         <v>1</v>
       </c>
@@ -14106,27 +14227,30 @@
       <c r="G30" s="176" t="s">
         <v>40</v>
       </c>
-      <c r="H30" s="175" t="s">
+      <c r="H30" s="176" t="s">
+        <v>350</v>
+      </c>
+      <c r="I30" s="175" t="s">
         <v>279</v>
       </c>
-      <c r="I30" s="177">
+      <c r="J30" s="177">
         <v>42876</v>
       </c>
-      <c r="J30" s="177">
+      <c r="K30" s="177">
         <v>43189</v>
       </c>
-      <c r="K30" s="178">
+      <c r="L30" s="178">
         <v>72.2</v>
       </c>
-      <c r="L30" s="179">
-        <f>K30*(20-1)</f>
+      <c r="M30" s="179">
+        <f>L30*(20-1)</f>
         <v>1371.8</v>
       </c>
-      <c r="M30" s="175" t="s">
+      <c r="N30" s="175" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="31" spans="1:16" s="180" customFormat="1">
+    <row r="31" spans="1:17" s="180" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="173">
         <v>1</v>
       </c>
@@ -14148,24 +14272,27 @@
       <c r="G31" s="176" t="s">
         <v>40</v>
       </c>
-      <c r="H31" s="175" t="s">
+      <c r="H31" s="176" t="s">
+        <v>351</v>
+      </c>
+      <c r="I31" s="175" t="s">
         <v>279</v>
       </c>
-      <c r="I31" s="177">
+      <c r="J31" s="177">
         <v>42886</v>
       </c>
-      <c r="J31" s="177">
+      <c r="K31" s="177">
         <v>43189</v>
       </c>
-      <c r="K31" s="178" t="s">
+      <c r="L31" s="178" t="s">
         <v>340</v>
       </c>
-      <c r="L31" s="179" t="s">
+      <c r="M31" s="179" t="s">
         <v>74</v>
       </c>
-      <c r="M31" s="175"/>
-    </row>
-    <row r="32" spans="1:16" s="180" customFormat="1">
+      <c r="N31" s="175"/>
+    </row>
+    <row r="32" spans="1:17" s="180" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="173">
         <v>1</v>
       </c>
@@ -14187,24 +14314,27 @@
       <c r="G32" s="176" t="s">
         <v>40</v>
       </c>
-      <c r="H32" s="175" t="s">
+      <c r="H32" s="176" t="s">
+        <v>351</v>
+      </c>
+      <c r="I32" s="175" t="s">
         <v>279</v>
       </c>
-      <c r="I32" s="177">
+      <c r="J32" s="177">
         <v>42910</v>
       </c>
-      <c r="J32" s="177">
+      <c r="K32" s="177">
         <v>43189</v>
       </c>
-      <c r="K32" s="178" t="s">
+      <c r="L32" s="178" t="s">
         <v>340</v>
       </c>
-      <c r="L32" s="179" t="s">
+      <c r="M32" s="179" t="s">
         <v>74</v>
       </c>
-      <c r="M32" s="175"/>
-    </row>
-    <row r="33" spans="1:13" s="180" customFormat="1">
+      <c r="N32" s="175"/>
+    </row>
+    <row r="33" spans="1:14" s="180" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="173">
         <v>1</v>
       </c>
@@ -14226,28 +14356,31 @@
       <c r="G33" s="176" t="s">
         <v>40</v>
       </c>
-      <c r="H33" s="175" t="s">
+      <c r="H33" s="176" t="s">
+        <v>350</v>
+      </c>
+      <c r="I33" s="175" t="s">
         <v>279</v>
       </c>
-      <c r="I33" s="177">
+      <c r="J33" s="177">
         <v>42882</v>
       </c>
-      <c r="J33" s="177">
+      <c r="K33" s="177">
         <v>43189</v>
       </c>
-      <c r="K33" s="178">
+      <c r="L33" s="178">
         <v>194</v>
       </c>
-      <c r="L33" s="179">
-        <f>K33*(20-1)</f>
+      <c r="M33" s="179">
+        <f>L33*(20-1)</f>
         <v>3686</v>
       </c>
-      <c r="M33" s="175" t="s">
+      <c r="N33" s="175" t="s">
         <v>282</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A21:O25">
+  <sortState ref="A21:P25">
     <sortCondition ref="A21"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -14256,7 +14389,7 @@
     <brk id="25" max="16383" man="1"/>
   </rowBreaks>
   <colBreaks count="1" manualBreakCount="1">
-    <brk id="12" max="1048575" man="1"/>
+    <brk id="13" max="1048575" man="1"/>
   </colBreaks>
   <legacyDrawing r:id="rId1"/>
   <extLst>

</xml_diff>

<commit_message>
process of moving analyses over to new directory
</commit_message>
<xml_diff>
--- a/Data/RNA-DNA-Isolation/DNA-extraction-data.xlsx
+++ b/Data/RNA-DNA-Isolation/DNA-extraction-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10309"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laura/Documents/roberts-lab/O.lurida_Stress/Data/RNA-DNA-Isolation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3869BF6B-C8F0-EB46-8493-764197712EDF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD7442F7-6ADE-244F-98AE-7C5B80A7D869}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13540" yWindow="460" windowWidth="10000" windowHeight="16920" tabRatio="1000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="17540" tabRatio="1000" firstSheet="8" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DNA Samples" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -3177,8 +3178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q58"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView showRuler="0" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5295,7 +5296,7 @@
       <c r="E58" s="16"/>
     </row>
   </sheetData>
-  <sortState ref="A27:O34">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A27:O34">
     <sortCondition ref="A27:A34"/>
     <sortCondition ref="C27:C34"/>
   </sortState>
@@ -5317,8 +5318,8 @@
   </sheetPr>
   <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView showRuler="0" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7580,7 +7581,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="G1" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
@@ -9035,7 +9036,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:S12">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S12">
     <sortCondition ref="D2:D12"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -10605,7 +10606,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:U25">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U25">
     <sortCondition ref="F2:F25"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -12099,7 +12100,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:S27">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S27">
     <sortCondition ref="E2:E27"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -12884,7 +12885,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:R15">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R15">
     <sortCondition ref="I2:I15"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -12904,8 +12905,8 @@
   </sheetPr>
   <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14392,7 +14393,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A21:P25">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A21:P25">
     <sortCondition ref="A21"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>